<commit_message>
chore: add entries to codebooks,, add analysis
</commit_message>
<xml_diff>
--- a/data/codebooks/codebook_columns.xlsx
+++ b/data/codebooks/codebook_columns.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20417"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeisegeierS\repos\github\sport-adverse-events\data\codebooks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDE342A-17B8-4629-944F-CD17B7BDF8A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="336">
   <si>
     <t>col_clean</t>
   </si>
@@ -1016,13 +1022,18 @@
   </si>
   <si>
     <t>Freitext_Observieren</t>
+  </si>
+  <si>
+    <t>[03.14.01] Adaptations intensity</t>
+  </si>
+  <si>
+    <t>[03.14.02] Adaptations duration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1041,7 +1052,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFc9211e"/>
+      <color rgb="FFC9211E"/>
       <name val="Cambria"/>
       <family val="2"/>
     </font>
@@ -1067,12 +1078,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFfac090"/>
+        <fgColor rgb="FFFAC090"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffff00"/>
+        <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1108,16 +1119,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1126,55 +1137,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1185,10 +1193,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1226,71 +1234,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1318,7 +1326,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1341,11 +1349,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1354,13 +1362,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1370,7 +1378,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1379,7 +1387,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1388,7 +1396,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1396,10 +1404,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1464,26 +1472,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="B67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G91" sqref="G91"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="11" width="73.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="42.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="53.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="53.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="73.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.6640625" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1506,7 +1516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row r="2" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -1518,12 +1528,13 @@
         <v>8</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="8">
-        <f>_xlfn.CONCAT(B2, , " ", E2)</f>
+      <c r="F2" s="8" t="str">
+        <f t="shared" ref="F2:F43" si="0">_xlfn.CONCAT(B2, , " ", E2)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -1535,12 +1546,13 @@
         <v>10</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="8">
-        <f>_xlfn.CONCAT(B3, , " ", E3)</f>
+      <c r="F3" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -1552,12 +1564,13 @@
         <v>12</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="8">
-        <f>_xlfn.CONCAT(B4, , " ", E4)</f>
+      <c r="F4" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -1569,12 +1582,13 @@
         <v>14</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="8">
-        <f>_xlfn.CONCAT(B5, , " ", E5)</f>
+      <c r="F5" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -1586,12 +1600,13 @@
         <v>16</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="8">
-        <f>_xlfn.CONCAT(B6, , " ", E6)</f>
+      <c r="F6" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
@@ -1603,12 +1618,13 @@
         <v>18</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="8">
-        <f>_xlfn.CONCAT(B7, , " ", E7)</f>
+      <c r="F7" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row r="8" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -1620,12 +1636,13 @@
         <v>20</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="8">
-        <f>_xlfn.CONCAT(B8, , " ", E8)</f>
+      <c r="F8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row r="9" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
@@ -1637,12 +1654,13 @@
         <v>22</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="8">
-        <f>_xlfn.CONCAT(B9, , " ", E9)</f>
+      <c r="F9" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row r="10" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
@@ -1654,12 +1672,13 @@
         <v>24</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="8">
-        <f>_xlfn.CONCAT(B10, , " ", E10)</f>
+      <c r="F10" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row r="11" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
@@ -1671,12 +1690,13 @@
         <v>26</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="8">
-        <f>_xlfn.CONCAT(B11, , " ", E11)</f>
+      <c r="F11" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
@@ -1688,12 +1708,13 @@
         <v>28</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="8">
-        <f>_xlfn.CONCAT(B12, , " ", E12)</f>
+      <c r="F12" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row r="13" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
@@ -1705,12 +1726,13 @@
         <v>30</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="8">
-        <f>_xlfn.CONCAT(B13, , " ", E13)</f>
+      <c r="F13" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row r="14" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
@@ -1722,12 +1744,13 @@
         <v>32</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="8">
-        <f>_xlfn.CONCAT(B14, , " ", E14)</f>
+      <c r="F14" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G14" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
@@ -1739,12 +1762,13 @@
         <v>34</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="8">
-        <f>_xlfn.CONCAT(B15, , " ", E15)</f>
+      <c r="F15" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G15" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row r="16" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>35</v>
       </c>
@@ -1756,12 +1780,13 @@
         <v>36</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="8">
-        <f>_xlfn.CONCAT(B16, , " ", E16)</f>
+      <c r="F16" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>37</v>
       </c>
@@ -1773,12 +1798,13 @@
         <v>38</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="8">
-        <f>_xlfn.CONCAT(B17, , " ", E17)</f>
+      <c r="F17" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>39</v>
       </c>
@@ -1790,12 +1816,13 @@
         <v>39</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="8">
-        <f>_xlfn.CONCAT(B18, , " ", E18)</f>
+      <c r="F18" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row r="19" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>40</v>
       </c>
@@ -1807,12 +1834,13 @@
         <v>40</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="8">
-        <f>_xlfn.CONCAT(B19, , " ", E19)</f>
+      <c r="F19" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row r="20" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>41</v>
       </c>
@@ -1824,12 +1852,13 @@
         <v>41</v>
       </c>
       <c r="E20" s="4"/>
-      <c r="F20" s="8">
-        <f>_xlfn.CONCAT(B20, , " ", E20)</f>
+      <c r="F20" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row r="21" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>42</v>
       </c>
@@ -1841,12 +1870,13 @@
         <v>43</v>
       </c>
       <c r="E21" s="4"/>
-      <c r="F21" s="8">
-        <f>_xlfn.CONCAT(B21, , " ", E21)</f>
+      <c r="F21" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>44</v>
       </c>
@@ -1858,12 +1888,13 @@
         <v>45</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="8">
-        <f>_xlfn.CONCAT(B22, , " ", E22)</f>
+      <c r="F22" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row r="23" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>46</v>
       </c>
@@ -1875,12 +1906,13 @@
         <v>47</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="F23" s="8">
-        <f>_xlfn.CONCAT(B23, , " ", E23)</f>
+      <c r="F23" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row r="24" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>48</v>
       </c>
@@ -1892,12 +1924,13 @@
         <v>49</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="8">
-        <f>_xlfn.CONCAT(B24, , " ", E24)</f>
+      <c r="F24" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row r="25" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>50</v>
       </c>
@@ -1909,12 +1942,13 @@
         <v>51</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="8">
-        <f>_xlfn.CONCAT(B25, , " ", E25)</f>
+      <c r="F25" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row r="26" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>52</v>
       </c>
@@ -1926,12 +1960,13 @@
         <v>53</v>
       </c>
       <c r="E26" s="4"/>
-      <c r="F26" s="8">
-        <f>_xlfn.CONCAT(B26, , " ", E26)</f>
+      <c r="F26" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row r="27" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>54</v>
       </c>
@@ -1943,12 +1978,13 @@
         <v>55</v>
       </c>
       <c r="E27" s="4"/>
-      <c r="F27" s="8">
-        <f>_xlfn.CONCAT(B27, , " ", E27)</f>
+      <c r="F27" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row r="28" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>56</v>
       </c>
@@ -1960,12 +1996,13 @@
         <v>57</v>
       </c>
       <c r="E28" s="4"/>
-      <c r="F28" s="8">
-        <f>_xlfn.CONCAT(B28, , " ", E28)</f>
+      <c r="F28" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G28" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row r="29" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>58</v>
       </c>
@@ -1977,12 +2014,13 @@
         <v>59</v>
       </c>
       <c r="E29" s="4"/>
-      <c r="F29" s="8">
-        <f>_xlfn.CONCAT(B29, , " ", E29)</f>
+      <c r="F29" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G29" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row r="30" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>60</v>
       </c>
@@ -1994,12 +2032,13 @@
         <v>61</v>
       </c>
       <c r="E30" s="4"/>
-      <c r="F30" s="8">
-        <f>_xlfn.CONCAT(B30, , " ", E30)</f>
+      <c r="F30" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G30" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+    <row r="31" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>62</v>
       </c>
@@ -2011,12 +2050,13 @@
         <v>63</v>
       </c>
       <c r="E31" s="4"/>
-      <c r="F31" s="8">
-        <f>_xlfn.CONCAT(B31, , " ", E31)</f>
+      <c r="F31" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G31" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+    <row r="32" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>64</v>
       </c>
@@ -2028,12 +2068,13 @@
         <v>65</v>
       </c>
       <c r="E32" s="4"/>
-      <c r="F32" s="8">
-        <f>_xlfn.CONCAT(B32, , " ", E32)</f>
+      <c r="F32" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G32" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+    <row r="33" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>66</v>
       </c>
@@ -2045,12 +2086,13 @@
         <v>67</v>
       </c>
       <c r="E33" s="4"/>
-      <c r="F33" s="8">
-        <f>_xlfn.CONCAT(B33, , " ", E33)</f>
+      <c r="F33" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G33" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+    <row r="34" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>68</v>
       </c>
@@ -2062,12 +2104,13 @@
         <v>69</v>
       </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="8">
-        <f>_xlfn.CONCAT(B34, , " ", E34)</f>
+      <c r="F34" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G34" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+    <row r="35" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>70</v>
       </c>
@@ -2079,12 +2122,13 @@
         <v>71</v>
       </c>
       <c r="E35" s="4"/>
-      <c r="F35" s="8">
-        <f>_xlfn.CONCAT(B35, , " ", E35)</f>
+      <c r="F35" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G35" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
+    <row r="36" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>72</v>
       </c>
@@ -2096,12 +2140,13 @@
         <v>73</v>
       </c>
       <c r="E36" s="4"/>
-      <c r="F36" s="8">
-        <f>_xlfn.CONCAT(B36, , " ", E36)</f>
+      <c r="F36" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G36" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+    <row r="37" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>74</v>
       </c>
@@ -2113,12 +2158,13 @@
         <v>75</v>
       </c>
       <c r="E37" s="4"/>
-      <c r="F37" s="8">
-        <f>_xlfn.CONCAT(B37, , " ", E37)</f>
+      <c r="F37" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G37" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
+    <row r="38" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>76</v>
       </c>
@@ -2130,12 +2176,13 @@
         <v>77</v>
       </c>
       <c r="E38" s="4"/>
-      <c r="F38" s="8">
-        <f>_xlfn.CONCAT(B38, , " ", E38)</f>
+      <c r="F38" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G38" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
+    <row r="39" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>78</v>
       </c>
@@ -2147,12 +2194,13 @@
         <v>79</v>
       </c>
       <c r="E39" s="4"/>
-      <c r="F39" s="8">
-        <f>_xlfn.CONCAT(B39, , " ", E39)</f>
+      <c r="F39" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G39" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
+    <row r="40" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>80</v>
       </c>
@@ -2164,12 +2212,13 @@
         <v>81</v>
       </c>
       <c r="E40" s="4"/>
-      <c r="F40" s="8">
-        <f>_xlfn.CONCAT(B40, , " ", E40)</f>
+      <c r="F40" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G40" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
+    <row r="41" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>82</v>
       </c>
@@ -2181,12 +2230,13 @@
         <v>83</v>
       </c>
       <c r="E41" s="4"/>
-      <c r="F41" s="8">
-        <f>_xlfn.CONCAT(B41, , " ", E41)</f>
+      <c r="F41" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G41" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
+    <row r="42" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>84</v>
       </c>
@@ -2198,12 +2248,13 @@
         <v>85</v>
       </c>
       <c r="E42" s="4"/>
-      <c r="F42" s="8">
-        <f>_xlfn.CONCAT(B42, , " ", E42)</f>
+      <c r="F42" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G42" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
+    <row r="43" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>86</v>
       </c>
@@ -2215,12 +2266,13 @@
         <v>87</v>
       </c>
       <c r="E43" s="4"/>
-      <c r="F43" s="8">
-        <f>_xlfn.CONCAT(B43, , " ", E43)</f>
+      <c r="F43" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G43" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
+    <row r="44" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>88</v>
       </c>
@@ -2234,14 +2286,15 @@
         <v>90</v>
       </c>
       <c r="E44" s="4"/>
-      <c r="F44" s="8">
-        <f>_xlfn.CONCAT(B44, , " ", D44)</f>
+      <c r="F44" s="8" t="str">
+        <f t="shared" ref="F44:F75" si="1">_xlfn.CONCAT(B44, , " ", D44)</f>
+        <v xml:space="preserve">[01.01] CTCAE </v>
       </c>
       <c r="G44" s="9" t="s">
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
+    <row r="45" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>92</v>
       </c>
@@ -2255,14 +2308,15 @@
         <v>94</v>
       </c>
       <c r="E45" s="7"/>
-      <c r="F45" s="8">
-        <f>_xlfn.CONCAT(B45, , " ", D45)</f>
+      <c r="F45" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[01.02] Datum_AE</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
+    <row r="46" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>96</v>
       </c>
@@ -2276,14 +2330,15 @@
         <v>30</v>
       </c>
       <c r="E46" s="4"/>
-      <c r="F46" s="8">
-        <f>_xlfn.CONCAT(B46, , " ", D46)</f>
+      <c r="F46" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[01.03] Sportassoziation</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
+    <row r="47" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>99</v>
       </c>
@@ -2297,12 +2352,13 @@
         <v>101</v>
       </c>
       <c r="E47" s="7"/>
-      <c r="F47" s="8">
-        <f>_xlfn.CONCAT(B47, , " ", D47)</f>
+      <c r="F47" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[02.01] Datum_Aufnahme</v>
       </c>
       <c r="G47" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
+    <row r="48" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>102</v>
       </c>
@@ -2316,14 +2372,15 @@
         <v>49</v>
       </c>
       <c r="E48" s="4"/>
-      <c r="F48" s="8">
-        <f>_xlfn.CONCAT(B48, , " ", D48)</f>
+      <c r="F48" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[02.02] Art</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>104</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
+    <row r="49" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>105</v>
       </c>
@@ -2337,14 +2394,15 @@
         <v>107</v>
       </c>
       <c r="E49" s="4"/>
-      <c r="F49" s="8">
-        <f>_xlfn.CONCAT(B49, , " ", D49)</f>
+      <c r="F49" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[02.03] Auslösser</v>
       </c>
       <c r="G49" s="9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
+    <row r="50" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>109</v>
       </c>
@@ -2358,14 +2416,15 @@
         <v>111</v>
       </c>
       <c r="E50" s="4"/>
-      <c r="F50" s="8">
-        <f>_xlfn.CONCAT(B50, , " ", D50)</f>
+      <c r="F50" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[02.04] Körperteil</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
+    <row r="51" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>113</v>
       </c>
@@ -2379,12 +2438,13 @@
         <v>115</v>
       </c>
       <c r="E51" s="4"/>
-      <c r="F51" s="8">
-        <f>_xlfn.CONCAT(B51, , " ", D51)</f>
+      <c r="F51" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.01.01] Schmerzen_Intensität</v>
       </c>
       <c r="G51" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25">
+    <row r="52" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>116</v>
       </c>
@@ -2398,12 +2458,13 @@
         <v>118</v>
       </c>
       <c r="E52" s="4"/>
-      <c r="F52" s="8">
-        <f>_xlfn.CONCAT(B52, , " ", D52)</f>
+      <c r="F52" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.01.02] Schmerzen_Dauer</v>
       </c>
       <c r="G52" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25">
+    <row r="53" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>119</v>
       </c>
@@ -2417,14 +2478,15 @@
         <v>121</v>
       </c>
       <c r="E53" s="4"/>
-      <c r="F53" s="8">
-        <f>_xlfn.CONCAT(B53, , " ", D53)</f>
+      <c r="F53" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.01] Schmerzen_Folge</v>
       </c>
       <c r="G53" s="9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25">
+    <row r="54" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>123</v>
       </c>
@@ -2438,12 +2500,13 @@
         <v>125</v>
       </c>
       <c r="E54" s="7"/>
-      <c r="F54" s="8">
-        <f>_xlfn.CONCAT(B54, , " ", D54)</f>
+      <c r="F54" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">[03.02.01] Krankenhaus_Intensität </v>
       </c>
       <c r="G54" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25">
+    <row r="55" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>126</v>
       </c>
@@ -2457,12 +2520,13 @@
         <v>128</v>
       </c>
       <c r="E55" s="7"/>
-      <c r="F55" s="8">
-        <f>_xlfn.CONCAT(B55, , " ", D55)</f>
+      <c r="F55" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.02.02] Krankenhaus_Dauer</v>
       </c>
       <c r="G55" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25">
+    <row r="56" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>129</v>
       </c>
@@ -2476,14 +2540,15 @@
         <v>131</v>
       </c>
       <c r="E56" s="4"/>
-      <c r="F56" s="8">
-        <f>_xlfn.CONCAT(B56, , " ", D56)</f>
+      <c r="F56" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.02] Krankenhaus_Folge</v>
       </c>
       <c r="G56" s="9" t="s">
         <v>132</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25">
+    <row r="57" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>133</v>
       </c>
@@ -2497,12 +2562,13 @@
         <v>135</v>
       </c>
       <c r="E57" s="4"/>
-      <c r="F57" s="8">
-        <f>_xlfn.CONCAT(B57, , " ", D57)</f>
+      <c r="F57" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.03.01] Med.Weiterbehandlung_Intensität</v>
       </c>
       <c r="G57" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25">
+    <row r="58" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>136</v>
       </c>
@@ -2516,12 +2582,13 @@
         <v>138</v>
       </c>
       <c r="E58" s="4"/>
-      <c r="F58" s="8">
-        <f>_xlfn.CONCAT(B58, , " ", D58)</f>
+      <c r="F58" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.03.02] Med.Weiterbehandlung_Dauer</v>
       </c>
       <c r="G58" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25">
+    <row r="59" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>139</v>
       </c>
@@ -2535,14 +2602,15 @@
         <v>141</v>
       </c>
       <c r="E59" s="4"/>
-      <c r="F59" s="8">
-        <f>_xlfn.CONCAT(B59, , " ", D59)</f>
+      <c r="F59" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.03] Med.Weiterbehandlung_Folge</v>
       </c>
       <c r="G59" s="9" t="s">
         <v>142</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="17.25">
+    <row r="60" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>143</v>
       </c>
@@ -2556,12 +2624,13 @@
         <v>145</v>
       </c>
       <c r="E60" s="7"/>
-      <c r="F60" s="8">
-        <f>_xlfn.CONCAT(B60, , " ", D60)</f>
+      <c r="F60" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.04.01] Therapieprotokoll_Intensität</v>
       </c>
       <c r="G60" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25">
+    <row r="61" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>146</v>
       </c>
@@ -2575,12 +2644,13 @@
         <v>148</v>
       </c>
       <c r="E61" s="7"/>
-      <c r="F61" s="8">
-        <f>_xlfn.CONCAT(B61, , " ", D61)</f>
+      <c r="F61" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.04.02] Therapieprotokoll_Dauer</v>
       </c>
       <c r="G61" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="17.25">
+    <row r="62" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>149</v>
       </c>
@@ -2594,14 +2664,15 @@
         <v>151</v>
       </c>
       <c r="E62" s="4"/>
-      <c r="F62" s="8">
-        <f>_xlfn.CONCAT(B62, , " ", D62)</f>
+      <c r="F62" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.04] Therapieprotokoll_Folge</v>
       </c>
       <c r="G62" s="9" t="s">
         <v>152</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="17.25">
+    <row r="63" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>153</v>
       </c>
@@ -2615,14 +2686,15 @@
         <v>155</v>
       </c>
       <c r="E63" s="4"/>
-      <c r="F63" s="8">
-        <f>_xlfn.CONCAT(B63, , " ", D63)</f>
+      <c r="F63" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.05] lebensnotwendigeIntenvention_Folge</v>
       </c>
       <c r="G63" s="9" t="s">
         <v>156</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="17.25">
+    <row r="64" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>157</v>
       </c>
@@ -2634,12 +2706,13 @@
         <v>159</v>
       </c>
       <c r="E64" s="7"/>
-      <c r="F64" s="8">
-        <f>_xlfn.CONCAT(B64, , " ", D64)</f>
+      <c r="F64" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.05.01] lebensnotwendigeIntenvention_Intensität</v>
       </c>
       <c r="G64" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="17.25">
+    <row r="65" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>160</v>
       </c>
@@ -2651,12 +2724,13 @@
         <v>162</v>
       </c>
       <c r="E65" s="7"/>
-      <c r="F65" s="8">
-        <f>_xlfn.CONCAT(B65, , " ", D65)</f>
+      <c r="F65" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.05.02] lebensnotwendigeIntenvention_Dauer</v>
       </c>
       <c r="G65" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="17.25">
+    <row r="66" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>163</v>
       </c>
@@ -2670,12 +2744,13 @@
         <v>165</v>
       </c>
       <c r="E66" s="7"/>
-      <c r="F66" s="8">
-        <f>_xlfn.CONCAT(B66, , " ", D66)</f>
+      <c r="F66" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.06.01] Pflege_Intensität</v>
       </c>
       <c r="G66" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="17.25">
+    <row r="67" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>166</v>
       </c>
@@ -2689,12 +2764,13 @@
         <v>168</v>
       </c>
       <c r="E67" s="7"/>
-      <c r="F67" s="8">
-        <f>_xlfn.CONCAT(B67, , " ", D67)</f>
+      <c r="F67" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.06.02] Pflege_Dauer</v>
       </c>
       <c r="G67" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="17.25">
+    <row r="68" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>169</v>
       </c>
@@ -2708,14 +2784,15 @@
         <v>171</v>
       </c>
       <c r="E68" s="4"/>
-      <c r="F68" s="8">
-        <f>_xlfn.CONCAT(B68, , " ", D68)</f>
+      <c r="F68" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.06] Pflege_Folge</v>
       </c>
       <c r="G68" s="9" t="s">
         <v>172</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="17.25">
+    <row r="69" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>173</v>
       </c>
@@ -2729,12 +2806,13 @@
         <v>175</v>
       </c>
       <c r="E69" s="7"/>
-      <c r="F69" s="8">
-        <f>_xlfn.CONCAT(B69, , " ", D69)</f>
+      <c r="F69" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.07.01] Medikamente_Dauer</v>
       </c>
       <c r="G69" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="17.25">
+    <row r="70" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>176</v>
       </c>
@@ -2748,12 +2826,13 @@
         <v>178</v>
       </c>
       <c r="E70" s="7"/>
-      <c r="F70" s="8">
-        <f>_xlfn.CONCAT(B70, , " ", D70)</f>
+      <c r="F70" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.07.02] Medikamente_Intensität</v>
       </c>
       <c r="G70" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="17.25">
+    <row r="71" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>179</v>
       </c>
@@ -2767,14 +2846,15 @@
         <v>181</v>
       </c>
       <c r="E71" s="4"/>
-      <c r="F71" s="8">
-        <f>_xlfn.CONCAT(B71, , " ", D71)</f>
+      <c r="F71" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.07] Medikamente_Folge</v>
       </c>
       <c r="G71" s="9" t="s">
         <v>182</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="17.25">
+    <row r="72" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>183</v>
       </c>
@@ -2788,14 +2868,15 @@
         <v>185</v>
       </c>
       <c r="E72" s="7"/>
-      <c r="F72" s="8">
-        <f>_xlfn.CONCAT(B72, , " ", D72)</f>
+      <c r="F72" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.08.01] Angst_Intensität</v>
       </c>
       <c r="G72" s="9" t="s">
         <v>186</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="17.25">
+    <row r="73" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>187</v>
       </c>
@@ -2809,12 +2890,13 @@
         <v>189</v>
       </c>
       <c r="E73" s="7"/>
-      <c r="F73" s="8">
-        <f>_xlfn.CONCAT(B73, , " ", D73)</f>
+      <c r="F73" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.08.02] Angst_Dauer</v>
       </c>
       <c r="G73" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="17.25">
+    <row r="74" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>190</v>
       </c>
@@ -2828,14 +2910,15 @@
         <v>192</v>
       </c>
       <c r="E74" s="4"/>
-      <c r="F74" s="8">
-        <f>_xlfn.CONCAT(B74, , " ", D74)</f>
+      <c r="F74" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.08] Angst_Folge</v>
       </c>
       <c r="G74" s="9" t="s">
         <v>193</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="17.25">
+    <row r="75" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>194</v>
       </c>
@@ -2849,12 +2932,13 @@
         <v>196</v>
       </c>
       <c r="E75" s="4"/>
-      <c r="F75" s="8">
-        <f>_xlfn.CONCAT(B75, , " ", D75)</f>
+      <c r="F75" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>[03.09.01] Strukturanpassung_Intensität</v>
       </c>
       <c r="G75" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="17.25">
+    <row r="76" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>197</v>
       </c>
@@ -2868,12 +2952,13 @@
         <v>199</v>
       </c>
       <c r="E76" s="4"/>
-      <c r="F76" s="8">
-        <f>_xlfn.CONCAT(B76, , " ", D76)</f>
+      <c r="F76" s="8" t="str">
+        <f t="shared" ref="F76:F107" si="2">_xlfn.CONCAT(B76, , " ", D76)</f>
+        <v>[03.09.02] Strukturanpassung_Dauer</v>
       </c>
       <c r="G76" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="17.25">
+    <row r="77" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>200</v>
       </c>
@@ -2887,14 +2972,15 @@
         <v>202</v>
       </c>
       <c r="E77" s="4"/>
-      <c r="F77" s="8">
-        <f>_xlfn.CONCAT(B77, , " ", D77)</f>
+      <c r="F77" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.09] Strukturanpassung_Folge</v>
       </c>
       <c r="G77" s="9" t="s">
         <v>203</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="17.25">
+    <row r="78" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>204</v>
       </c>
@@ -2908,14 +2994,15 @@
         <v>206</v>
       </c>
       <c r="E78" s="4"/>
-      <c r="F78" s="8">
-        <f>_xlfn.CONCAT(B78, , " ", D78)</f>
+      <c r="F78" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.10.01] Freigabe_OK</v>
       </c>
       <c r="G78" s="9" t="s">
         <v>207</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="17.25">
+    <row r="79" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>208</v>
       </c>
@@ -2929,14 +3016,15 @@
         <v>210</v>
       </c>
       <c r="E79" s="4"/>
-      <c r="F79" s="8">
-        <f>_xlfn.CONCAT(B79, , " ", D79)</f>
+      <c r="F79" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.10.02] Freigabe_Wer</v>
       </c>
       <c r="G79" s="9" t="s">
         <v>211</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="17.25">
+    <row r="80" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>212</v>
       </c>
@@ -2950,14 +3038,15 @@
         <v>214</v>
       </c>
       <c r="E80" s="4"/>
-      <c r="F80" s="8">
-        <f>_xlfn.CONCAT(B80, , " ", D80)</f>
+      <c r="F80" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.10] Freigabe_Folge</v>
       </c>
       <c r="G80" s="9" t="s">
         <v>215</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="17.25">
+    <row r="81" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>216</v>
       </c>
@@ -2971,12 +3060,13 @@
         <v>218</v>
       </c>
       <c r="E81" s="4"/>
-      <c r="F81" s="8">
-        <f>_xlfn.CONCAT(B81, , " ", D81)</f>
+      <c r="F81" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.11.01] PECH_Intensität</v>
       </c>
       <c r="G81" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="17.25">
+    <row r="82" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>219</v>
       </c>
@@ -2990,12 +3080,13 @@
         <v>221</v>
       </c>
       <c r="E82" s="4"/>
-      <c r="F82" s="8">
-        <f>_xlfn.CONCAT(B82, , " ", D82)</f>
+      <c r="F82" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.11.02] PECH_Folge</v>
       </c>
       <c r="G82" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="17.25">
+    <row r="83" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>222</v>
       </c>
@@ -3009,14 +3100,15 @@
         <v>221</v>
       </c>
       <c r="E83" s="4"/>
-      <c r="F83" s="8">
-        <f>_xlfn.CONCAT(B83, , " ", D83)</f>
+      <c r="F83" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.11] PECH_Folge</v>
       </c>
       <c r="G83" s="9" t="s">
         <v>224</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="17.25">
+    <row r="84" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>225</v>
       </c>
@@ -3030,12 +3122,13 @@
         <v>227</v>
       </c>
       <c r="E84" s="7"/>
-      <c r="F84" s="8">
-        <f>_xlfn.CONCAT(B84, , " ", D84)</f>
+      <c r="F84" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.12.01] Observierung_Intensität</v>
       </c>
       <c r="G84" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
+    <row r="85" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>228</v>
       </c>
@@ -3049,12 +3142,13 @@
         <v>230</v>
       </c>
       <c r="E85" s="7"/>
-      <c r="F85" s="8">
-        <f>_xlfn.CONCAT(B85, , " ", D85)</f>
+      <c r="F85" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.12.02] Observierung_Dauer</v>
       </c>
       <c r="G85" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
+    <row r="86" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>231</v>
       </c>
@@ -3068,14 +3162,15 @@
         <v>233</v>
       </c>
       <c r="E86" s="4"/>
-      <c r="F86" s="8">
-        <f>_xlfn.CONCAT(B86, , " ", D86)</f>
+      <c r="F86" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.12] Observierung_Folge</v>
       </c>
       <c r="G86" s="9" t="s">
         <v>234</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
+    <row r="87" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>235</v>
       </c>
@@ -3089,14 +3184,15 @@
         <v>237</v>
       </c>
       <c r="E87" s="4"/>
-      <c r="F87" s="8">
-        <f>_xlfn.CONCAT(B87, , " ", D87)</f>
+      <c r="F87" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.13.01] Ende_vs_Pause</v>
       </c>
       <c r="G87" s="9" t="s">
         <v>238</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
+    <row r="88" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>239</v>
       </c>
@@ -3110,12 +3206,13 @@
         <v>241</v>
       </c>
       <c r="E88" s="4"/>
-      <c r="F88" s="8">
-        <f>_xlfn.CONCAT(B88, , " ", D88)</f>
+      <c r="F88" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.13.02] Pause_Intensität</v>
       </c>
       <c r="G88" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
+    <row r="89" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>242</v>
       </c>
@@ -3129,14 +3226,15 @@
         <v>244</v>
       </c>
       <c r="E89" s="4"/>
-      <c r="F89" s="8">
-        <f>_xlfn.CONCAT(B89, , " ", D89)</f>
+      <c r="F89" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.13] Stoppung_Folge</v>
       </c>
       <c r="G89" s="9" t="s">
         <v>245</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
+    <row r="90" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>246</v>
       </c>
@@ -3150,12 +3248,15 @@
         <v>248</v>
       </c>
       <c r="E90" s="4"/>
-      <c r="F90" s="8">
-        <f>_xlfn.CONCAT(B90, , " ", D90)</f>
-      </c>
-      <c r="G90" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
+      <c r="F90" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.14.01] Anpassung_Intensität</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>249</v>
       </c>
@@ -3169,12 +3270,15 @@
         <v>251</v>
       </c>
       <c r="E91" s="4"/>
-      <c r="F91" s="8">
-        <f>_xlfn.CONCAT(B91, , " ", D91)</f>
-      </c>
-      <c r="G91" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
+      <c r="F91" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.14.02] Anpassung_Dauer</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>252</v>
       </c>
@@ -3188,14 +3292,15 @@
         <v>254</v>
       </c>
       <c r="E92" s="4"/>
-      <c r="F92" s="8">
-        <f>_xlfn.CONCAT(B92, , " ", D92)</f>
+      <c r="F92" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.14] Anpassung_Folge</v>
       </c>
       <c r="G92" s="9" t="s">
         <v>255</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
+    <row r="93" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>256</v>
       </c>
@@ -3209,12 +3314,13 @@
         <v>258</v>
       </c>
       <c r="E93" s="7"/>
-      <c r="F93" s="8">
-        <f>_xlfn.CONCAT(B93, , " ", D93)</f>
+      <c r="F93" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.15.01] Trost_Intesität</v>
       </c>
       <c r="G93" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
+    <row r="94" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>259</v>
       </c>
@@ -3228,12 +3334,13 @@
         <v>261</v>
       </c>
       <c r="E94" s="7"/>
-      <c r="F94" s="8">
-        <f>_xlfn.CONCAT(B94, , " ", D94)</f>
+      <c r="F94" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.15.02] Trost_Dauer</v>
       </c>
       <c r="G94" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5">
+    <row r="95" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>262</v>
       </c>
@@ -3247,12 +3354,13 @@
         <v>264</v>
       </c>
       <c r="E95" s="4"/>
-      <c r="F95" s="8">
-        <f>_xlfn.CONCAT(B95, , " ", D95)</f>
+      <c r="F95" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.15] Trost_Folge</v>
       </c>
       <c r="G95" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5">
+    <row r="96" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>265</v>
       </c>
@@ -3266,14 +3374,15 @@
         <v>267</v>
       </c>
       <c r="E96" s="4"/>
-      <c r="F96" s="8">
-        <f>_xlfn.CONCAT(B96, , " ", D96)</f>
+      <c r="F96" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.16] Tod_Folge</v>
       </c>
       <c r="G96" s="9" t="s">
         <v>268</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5">
+    <row r="97" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>269</v>
       </c>
@@ -3287,12 +3396,13 @@
         <v>271</v>
       </c>
       <c r="E97" s="7"/>
-      <c r="F97" s="8">
-        <f>_xlfn.CONCAT(B97, , " ", D97)</f>
+      <c r="F97" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.17.01] ADL_Intensität</v>
       </c>
       <c r="G97" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
+    <row r="98" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>272</v>
       </c>
@@ -3306,12 +3416,13 @@
         <v>274</v>
       </c>
       <c r="E98" s="7"/>
-      <c r="F98" s="8">
-        <f>_xlfn.CONCAT(B98, , " ", D98)</f>
+      <c r="F98" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.17.02] ADL_Dauer</v>
       </c>
       <c r="G98" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
+    <row r="99" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>275</v>
       </c>
@@ -3325,12 +3436,13 @@
         <v>277</v>
       </c>
       <c r="E99" s="4"/>
-      <c r="F99" s="8">
-        <f>_xlfn.CONCAT(B99, , " ", D99)</f>
+      <c r="F99" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.17] ADL_Einschränkungen</v>
       </c>
       <c r="G99" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5">
+    <row r="100" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>278</v>
       </c>
@@ -3344,12 +3456,13 @@
         <v>280</v>
       </c>
       <c r="E100" s="7"/>
-      <c r="F100" s="8">
-        <f>_xlfn.CONCAT(B100, , " ", D100)</f>
+      <c r="F100" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[03.18] Freitext_Folgen</v>
       </c>
       <c r="G100" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5">
+    <row r="101" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>281</v>
       </c>
@@ -3363,14 +3476,15 @@
         <v>38</v>
       </c>
       <c r="E101" s="4"/>
-      <c r="F101" s="8">
-        <f>_xlfn.CONCAT(B101, , " ", D101)</f>
+      <c r="F101" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[05.01] Therapiephase</v>
       </c>
       <c r="G101" s="9" t="s">
         <v>283</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5">
+    <row r="102" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>284</v>
       </c>
@@ -3384,14 +3498,15 @@
         <v>34</v>
       </c>
       <c r="E102" s="4"/>
-      <c r="F102" s="8">
-        <f>_xlfn.CONCAT(B102, , " ", D102)</f>
+      <c r="F102" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[05.02] Gruppengröße</v>
       </c>
       <c r="G102" s="9" t="s">
         <v>286</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="19.5">
+    <row r="103" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>287</v>
       </c>
@@ -3405,14 +3520,15 @@
         <v>81</v>
       </c>
       <c r="E103" s="4"/>
-      <c r="F103" s="8">
-        <f>_xlfn.CONCAT(B103, , " ", D103)</f>
+      <c r="F103" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[05.03] Alter</v>
       </c>
       <c r="G103" s="9" t="s">
         <v>289</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="19.5">
+    <row r="104" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>290</v>
       </c>
@@ -3426,14 +3542,15 @@
         <v>28</v>
       </c>
       <c r="E104" s="4"/>
-      <c r="F104" s="8">
-        <f>_xlfn.CONCAT(B104, , " ", D104)</f>
+      <c r="F104" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[05.04] Online</v>
       </c>
       <c r="G104" s="9" t="s">
         <v>292</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="19.5">
+    <row r="105" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>293</v>
       </c>
@@ -3447,14 +3564,15 @@
         <v>26</v>
       </c>
       <c r="E105" s="4"/>
-      <c r="F105" s="8">
-        <f>_xlfn.CONCAT(B105, , " ", D105)</f>
+      <c r="F105" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[05.05] Testung</v>
       </c>
       <c r="G105" s="9" t="s">
         <v>295</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="19.5">
+    <row r="106" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>296</v>
       </c>
@@ -3468,14 +3586,15 @@
         <v>32</v>
       </c>
       <c r="E106" s="4"/>
-      <c r="F106" s="8">
-        <f>_xlfn.CONCAT(B106, , " ", D106)</f>
+      <c r="F106" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[05.06] Setting</v>
       </c>
       <c r="G106" s="9" t="s">
         <v>298</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="19.5">
+    <row r="107" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>299</v>
       </c>
@@ -3489,14 +3608,15 @@
         <v>301</v>
       </c>
       <c r="E107" s="4"/>
-      <c r="F107" s="8">
-        <f>_xlfn.CONCAT(B107, , " ", D107)</f>
+      <c r="F107" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>[05.07] Motorik</v>
       </c>
       <c r="G107" s="9" t="s">
         <v>302</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="19.5">
+    <row r="108" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>303</v>
       </c>
@@ -3510,14 +3630,15 @@
         <v>36</v>
       </c>
       <c r="E108" s="4"/>
-      <c r="F108" s="8">
-        <f>_xlfn.CONCAT(B108, , " ", D108)</f>
+      <c r="F108" s="8" t="str">
+        <f t="shared" ref="F108:F118" si="3">_xlfn.CONCAT(B108, , " ", D108)</f>
+        <v>[05.08] Hälfte</v>
       </c>
       <c r="G108" s="9" t="s">
         <v>305</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="19.5">
+    <row r="109" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>306</v>
       </c>
@@ -3531,14 +3652,15 @@
         <v>79</v>
       </c>
       <c r="E109" s="4"/>
-      <c r="F109" s="8">
-        <f>_xlfn.CONCAT(B109, , " ", D109)</f>
+      <c r="F109" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">[05.09] Trainingszustand </v>
       </c>
       <c r="G109" s="9" t="s">
         <v>308</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="19.5">
+    <row r="110" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>309</v>
       </c>
@@ -3552,12 +3674,13 @@
         <v>311</v>
       </c>
       <c r="E110" s="7"/>
-      <c r="F110" s="8">
-        <f>_xlfn.CONCAT(B110, , " ", D110)</f>
+      <c r="F110" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>[06.01] Freitext_Auslöser</v>
       </c>
       <c r="G110" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="19.5">
+    <row r="111" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>312</v>
       </c>
@@ -3571,12 +3694,13 @@
         <v>314</v>
       </c>
       <c r="E111" s="7"/>
-      <c r="F111" s="8">
-        <f>_xlfn.CONCAT(B111, , " ", D111)</f>
+      <c r="F111" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>[06.11] Freitext_Anmerkung</v>
       </c>
       <c r="G111" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="19.5">
+    <row r="112" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>315</v>
       </c>
@@ -3590,12 +3714,13 @@
         <v>24</v>
       </c>
       <c r="E112" s="7"/>
-      <c r="F112" s="8">
-        <f>_xlfn.CONCAT(B112, , " ", D112)</f>
+      <c r="F112" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>[06.12] Freitext_Sonstiges</v>
       </c>
       <c r="G112" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="19.5">
+    <row r="113" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>317</v>
       </c>
@@ -3609,12 +3734,13 @@
         <v>8</v>
       </c>
       <c r="E113" s="7"/>
-      <c r="F113" s="8">
-        <f>_xlfn.CONCAT(B113, , " ", D113)</f>
+      <c r="F113" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>[07.01] Standort</v>
       </c>
       <c r="G113" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="19.5">
+    <row r="114" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>319</v>
       </c>
@@ -3628,12 +3754,13 @@
         <v>321</v>
       </c>
       <c r="E114" s="4"/>
-      <c r="F114" s="8">
-        <f>_xlfn.CONCAT(B114, , " ", D114)</f>
+      <c r="F114" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>[07.02] Einheiten</v>
       </c>
       <c r="G114" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="19.5">
+    <row r="115" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>322</v>
       </c>
@@ -3647,12 +3774,13 @@
         <v>324</v>
       </c>
       <c r="E115" s="7"/>
-      <c r="F115" s="8">
-        <f>_xlfn.CONCAT(B115, , " ", D115)</f>
+      <c r="F115" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>[07.03] Frteitext_med. Weiterbehandlung</v>
       </c>
       <c r="G115" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="19.5">
+    <row r="116" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>325</v>
       </c>
@@ -3666,12 +3794,13 @@
         <v>327</v>
       </c>
       <c r="E116" s="7"/>
-      <c r="F116" s="8">
-        <f>_xlfn.CONCAT(B116, , " ", D116)</f>
+      <c r="F116" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>[07.04] Freitext_Medikaments</v>
       </c>
       <c r="G116" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="19.5">
+    <row r="117" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>328</v>
       </c>
@@ -3685,12 +3814,13 @@
         <v>330</v>
       </c>
       <c r="E117" s="7"/>
-      <c r="F117" s="8">
-        <f>_xlfn.CONCAT(B117, , " ", D117)</f>
+      <c r="F117" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>[07.05] Freitext_Expertise</v>
       </c>
       <c r="G117" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="19.5">
+    <row r="118" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>331</v>
       </c>
@@ -3704,8 +3834,9 @@
         <v>333</v>
       </c>
       <c r="E118" s="7"/>
-      <c r="F118" s="8">
-        <f>_xlfn.CONCAT(B118, , " ", D118)</f>
+      <c r="F118" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>[07.07] Freitext_Observieren</v>
       </c>
       <c r="G118" s="9"/>
     </row>

</xml_diff>